<commit_message>
work on presentation and DAVID analysis
</commit_message>
<xml_diff>
--- a/all the important files/Initial genes.xlsx
+++ b/all the important files/Initial genes.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phenopedia" sheetId="1" r:id="rId1"/>
     <sheet name="PubMed" sheetId="3" r:id="rId2"/>
+    <sheet name="Combined" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PubMed!$A$1:$R$220</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="1322">
   <si>
     <t>Associated Gene</t>
   </si>
@@ -4084,7 +4085,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4391,8 +4413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6378,9 +6400,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18565,22 +18587,1583 @@
   </sheetData>
   <autoFilter ref="A1:R220"/>
   <conditionalFormatting sqref="F2:F220">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Q220">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="cataract">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="cataract">
       <formula>NOT(ISERROR(SEARCH("cataract",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:R220">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="cataract">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="cataract">
       <formula>NOT(ISERROR(SEARCH("cataract",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A307"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A307" sqref="A1:A307"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A163:A307">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A163:A307">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A163:A307">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="cataract">
+      <formula>NOT(ISERROR(SEARCH("cataract",A163)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>